<commit_message>
check in the latest version
</commit_message>
<xml_diff>
--- a/Practice statistics/LeetcodeQuestions May 9 2018 Last 12 months.xlsx
+++ b/Practice statistics/LeetcodeQuestions May 9 2018 Last 12 months.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Last 12 months May 9 2018 " sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -232,13 +232,16 @@
   </si>
   <si>
     <t>11 months, 3 weeks ago</t>
+  </si>
+  <si>
+    <t>Julia submitted those algorithm last 12 months. :-)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +255,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +297,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -402,9 +427,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -430,6 +454,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,6 +519,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -571,10 +598,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="F9:H52" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="F9:H52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:D52" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="B9:D52"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="2">
+      <calculatedColumnFormula>ROW() - 10</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="2" name="Name" dataDxfId="1"/>
     <tableColumn id="3" name="Date time" dataDxfId="0"/>
   </tableColumns>
@@ -869,417 +898,559 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F5:H52"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H52"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="64.5703125" customWidth="1"/>
-    <col min="8" max="8" width="37" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="1">
+    <row r="2" spans="2:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D7" s="16">
         <f ca="1">NOW()</f>
-        <v>43229.59838275463</v>
-      </c>
-    </row>
-    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F9" s="2" t="s">
+        <v>43229.618686226851</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="5"/>
-      <c r="G10" s="6" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <f t="shared" ref="B10:B52" si="0">ROW() - 10</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F11" s="5"/>
-      <c r="G11" s="8" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F12" s="5"/>
-      <c r="G12" s="8" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="5"/>
-      <c r="G13" s="6" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="5"/>
-      <c r="G14" s="6" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="5"/>
-      <c r="G15" s="8" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="5"/>
-      <c r="G16" s="8" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="5"/>
-      <c r="G17" s="6" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F18" s="5"/>
-      <c r="G18" s="8" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="5"/>
-      <c r="G19" s="8" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="5"/>
-      <c r="G20" s="8" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="5"/>
-      <c r="G21" s="10" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="5"/>
-      <c r="G22" s="8" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="5"/>
-      <c r="G23" s="8" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="5"/>
-      <c r="G24" s="6" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="5"/>
-      <c r="G25" s="12" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="5"/>
-      <c r="G26" s="6" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="5"/>
-      <c r="G27" s="6" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="5"/>
-      <c r="G28" s="8" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="5"/>
-      <c r="G29" s="6" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="5"/>
-      <c r="G30" s="12" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="5"/>
-      <c r="G31" s="8" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F32" s="5"/>
-      <c r="G32" s="10" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F33" s="5"/>
-      <c r="G33" s="6" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F34" s="5"/>
-      <c r="G34" s="10" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F35" s="5"/>
-      <c r="G35" s="10" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="5"/>
-      <c r="G36" s="12" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F37" s="5"/>
-      <c r="G37" s="10" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F38" s="5"/>
-      <c r="G38" s="10" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F39" s="5"/>
-      <c r="G39" s="12" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F40" s="5"/>
-      <c r="G40" s="10" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F41" s="5"/>
-      <c r="G41" s="8" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F42" s="5"/>
-      <c r="G42" s="10" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F43" s="5"/>
-      <c r="G43" s="10" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="5"/>
-      <c r="G44" s="10" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H44" s="13"/>
-    </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F45" s="5"/>
-      <c r="G45" s="10" t="s">
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H45" s="13"/>
-    </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="5"/>
-      <c r="G46" s="12" t="s">
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F47" s="5"/>
-      <c r="G47" s="6" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="4">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F48" s="5"/>
-      <c r="G48" s="12" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H48" s="13"/>
-    </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F49" s="5"/>
-      <c r="G49" s="8" t="s">
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H49" s="13"/>
-    </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F50" s="5"/>
-      <c r="G50" s="12" t="s">
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="H50" s="7" t="s">
+      <c r="D50" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F51" s="5"/>
-      <c r="G51" s="8" t="s">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F52" s="14"/>
-      <c r="G52" s="15" t="s">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="13">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="D52" s="15" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="91" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="57" max="16383" man="1"/>
+  </rowBreaks>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>